<commit_message>
correct some upper values of solar heat gain ratio
</commit_message>
<xml_diff>
--- a/_03_HCLoad_and_Envelope/EnvelopePerformanceSimpleTestCase.xlsx
+++ b/_03_HCLoad_and_Envelope/EnvelopePerformanceSimpleTestCase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11745"/>
@@ -10,7 +10,7 @@
     <sheet name="定義表" sheetId="1" r:id="rId1"/>
     <sheet name="規定値の検討" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1176,6 +1176,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.000"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -1456,7 +1459,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1515,6 +1518,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1936,14 +1940,14 @@
   </sheetPr>
   <dimension ref="B1:BQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="14" ySplit="3" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="14" ySplit="3" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P39" sqref="P39"/>
+      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="1.625" customWidth="1"/>
     <col min="2" max="2" width="38.875" bestFit="1" customWidth="1"/>
@@ -5224,8 +5228,8 @@
       <c r="J27" s="2">
         <v>0</v>
       </c>
-      <c r="K27" s="2">
-        <v>99.998999999999995</v>
+      <c r="K27" s="38">
+        <v>1</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>30</v>
@@ -5417,8 +5421,8 @@
       <c r="J28" s="2">
         <v>0</v>
       </c>
-      <c r="K28" s="2">
-        <v>99.998999999999995</v>
+      <c r="K28" s="38">
+        <v>1</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>30</v>
@@ -5880,8 +5884,8 @@
       <c r="J31" s="2">
         <v>0</v>
       </c>
-      <c r="K31" s="2">
-        <v>9.9990000000000006</v>
+      <c r="K31" s="38">
+        <v>1</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>30</v>
@@ -5981,8 +5985,8 @@
       <c r="J32" s="2">
         <v>0</v>
       </c>
-      <c r="K32" s="2">
-        <v>9.9990000000000006</v>
+      <c r="K32" s="38">
+        <v>1</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>30</v>
@@ -6569,7 +6573,7 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.649999999999999"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="9" style="10"/>
     <col min="2" max="2" width="27.875" style="10" customWidth="1"/>

</xml_diff>